<commit_message>
Requête POST lorsque boutons sont pressés
</commit_message>
<xml_diff>
--- a/Docs/EnzoRoy_Planning_Taches.xlsx
+++ b/Docs/EnzoRoy_Planning_Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoroy/Desktop/EnzoRoy_TPI/BotCleaner/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{632FCBDB-1B3F-954B-AAAE-09D299B8BD2C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C7F08-A316-8F4B-B524-5E30809A089B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="1" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="2" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
   <si>
     <t>Date</t>
   </si>
@@ -207,6 +207,21 @@
   </si>
   <si>
     <t>utilisation de flask pour le flux video -&gt; mjpeg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">page web </t>
+  </si>
+  <si>
+    <t>telecommande</t>
+  </si>
+  <si>
+    <t>ajout de la telecommande sur la page web</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation de la ge web </t>
+  </si>
+  <si>
+    <t>Total J2</t>
   </si>
 </sst>
 </file>
@@ -279,7 +294,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -673,11 +688,57 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="90">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -782,59 +843,11 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -845,6 +858,78 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="16" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1173,145 +1258,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="64" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="66">
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="72">
         <v>43592</v>
       </c>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="73"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="69" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="70" t="s">
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="71"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="66">
         <v>1</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="60">
+      <c r="C5" s="67"/>
+      <c r="D5" s="66">
         <v>2</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="60">
+      <c r="E5" s="67"/>
+      <c r="F5" s="66">
         <v>3</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="60">
+      <c r="G5" s="67"/>
+      <c r="H5" s="66">
         <v>4</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="60">
+      <c r="I5" s="67"/>
+      <c r="J5" s="66">
         <v>5</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="60">
+      <c r="K5" s="67"/>
+      <c r="L5" s="66">
         <v>6</v>
       </c>
-      <c r="M5" s="61"/>
-      <c r="N5" s="60">
+      <c r="M5" s="67"/>
+      <c r="N5" s="66">
         <v>7</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="60">
+      <c r="O5" s="67"/>
+      <c r="P5" s="66">
         <v>8</v>
       </c>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="60">
+      <c r="Q5" s="67"/>
+      <c r="R5" s="66">
         <v>9</v>
       </c>
-      <c r="S5" s="61"/>
-      <c r="T5" s="60">
+      <c r="S5" s="67"/>
+      <c r="T5" s="66">
         <v>10</v>
       </c>
-      <c r="U5" s="61"/>
-      <c r="V5" s="60">
+      <c r="U5" s="67"/>
+      <c r="V5" s="66">
         <v>11</v>
       </c>
-      <c r="W5" s="61"/>
+      <c r="W5" s="67"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -1710,6 +1795,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="P5:Q5"/>
+    <mergeCell ref="R5:S5"/>
+    <mergeCell ref="T5:U5"/>
+    <mergeCell ref="V5:W5"/>
     <mergeCell ref="L5:M5"/>
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="B2:E2"/>
@@ -1726,10 +1815,6 @@
     <mergeCell ref="H5:I5"/>
     <mergeCell ref="J5:K5"/>
     <mergeCell ref="N5:O5"/>
-    <mergeCell ref="P5:Q5"/>
-    <mergeCell ref="R5:S5"/>
-    <mergeCell ref="T5:U5"/>
-    <mergeCell ref="V5:W5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1739,8 +1824,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779F402-4327-4345-BFB9-00C0C178FF50}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1750,145 +1835,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
-      <c r="E1" s="62"/>
-      <c r="F1" s="62"/>
-      <c r="G1" s="62"/>
-      <c r="H1" s="62"/>
-      <c r="I1" s="62"/>
-      <c r="J1" s="62"/>
-      <c r="K1" s="62"/>
-      <c r="L1" s="62"/>
-      <c r="M1" s="62"/>
-      <c r="N1" s="62"/>
-      <c r="O1" s="62"/>
-      <c r="P1" s="62"/>
-      <c r="Q1" s="62"/>
-      <c r="R1" s="62"/>
-      <c r="S1" s="62"/>
-      <c r="T1" s="62"/>
-      <c r="U1" s="62"/>
-      <c r="V1" s="62"/>
-      <c r="W1" s="62"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="68"/>
+      <c r="J1" s="68"/>
+      <c r="K1" s="68"/>
+      <c r="L1" s="68"/>
+      <c r="M1" s="68"/>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+      <c r="V1" s="68"/>
+      <c r="W1" s="68"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="69" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="64"/>
-      <c r="E2" s="64"/>
-      <c r="F2" s="65" t="s">
+      <c r="C2" s="70"/>
+      <c r="D2" s="70"/>
+      <c r="E2" s="70"/>
+      <c r="F2" s="71" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="65"/>
-      <c r="H2" s="65"/>
-      <c r="I2" s="65"/>
-      <c r="J2" s="65"/>
-      <c r="K2" s="65"/>
-      <c r="L2" s="65"/>
-      <c r="M2" s="64" t="s">
+      <c r="G2" s="71"/>
+      <c r="H2" s="71"/>
+      <c r="I2" s="71"/>
+      <c r="J2" s="71"/>
+      <c r="K2" s="71"/>
+      <c r="L2" s="71"/>
+      <c r="M2" s="70" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="64"/>
-      <c r="O2" s="64"/>
-      <c r="P2" s="64"/>
-      <c r="Q2" s="66">
+      <c r="N2" s="70"/>
+      <c r="O2" s="70"/>
+      <c r="P2" s="70"/>
+      <c r="Q2" s="72">
         <v>43592</v>
       </c>
-      <c r="R2" s="66"/>
-      <c r="S2" s="66"/>
-      <c r="T2" s="66"/>
-      <c r="U2" s="66"/>
-      <c r="V2" s="66"/>
-      <c r="W2" s="67"/>
+      <c r="R2" s="72"/>
+      <c r="S2" s="72"/>
+      <c r="T2" s="72"/>
+      <c r="U2" s="72"/>
+      <c r="V2" s="72"/>
+      <c r="W2" s="73"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="68" t="s">
+      <c r="B3" s="74" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="69"/>
-      <c r="D3" s="69"/>
-      <c r="E3" s="69"/>
-      <c r="F3" s="70" t="s">
+      <c r="C3" s="75"/>
+      <c r="D3" s="75"/>
+      <c r="E3" s="75"/>
+      <c r="F3" s="76" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="70"/>
-      <c r="H3" s="70"/>
-      <c r="I3" s="70"/>
-      <c r="J3" s="70"/>
-      <c r="K3" s="70"/>
-      <c r="L3" s="70"/>
-      <c r="M3" s="69" t="s">
+      <c r="G3" s="76"/>
+      <c r="H3" s="76"/>
+      <c r="I3" s="76"/>
+      <c r="J3" s="76"/>
+      <c r="K3" s="76"/>
+      <c r="L3" s="76"/>
+      <c r="M3" s="75" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="69"/>
-      <c r="O3" s="69"/>
-      <c r="P3" s="69"/>
-      <c r="Q3" s="70" t="s">
+      <c r="N3" s="75"/>
+      <c r="O3" s="75"/>
+      <c r="P3" s="75"/>
+      <c r="Q3" s="76" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="70"/>
-      <c r="S3" s="70"/>
-      <c r="T3" s="70"/>
-      <c r="U3" s="70"/>
-      <c r="V3" s="70"/>
-      <c r="W3" s="71"/>
+      <c r="R3" s="76"/>
+      <c r="S3" s="76"/>
+      <c r="T3" s="76"/>
+      <c r="U3" s="76"/>
+      <c r="V3" s="76"/>
+      <c r="W3" s="77"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="60">
+      <c r="B5" s="66">
         <v>1</v>
       </c>
-      <c r="C5" s="61"/>
-      <c r="D5" s="60">
+      <c r="C5" s="67"/>
+      <c r="D5" s="66">
         <v>2</v>
       </c>
-      <c r="E5" s="61"/>
-      <c r="F5" s="60">
+      <c r="E5" s="67"/>
+      <c r="F5" s="66">
         <v>3</v>
       </c>
-      <c r="G5" s="61"/>
-      <c r="H5" s="60">
+      <c r="G5" s="67"/>
+      <c r="H5" s="66">
         <v>4</v>
       </c>
-      <c r="I5" s="61"/>
-      <c r="J5" s="60">
+      <c r="I5" s="67"/>
+      <c r="J5" s="66">
         <v>5</v>
       </c>
-      <c r="K5" s="61"/>
-      <c r="L5" s="60">
+      <c r="K5" s="67"/>
+      <c r="L5" s="66">
         <v>6</v>
       </c>
-      <c r="M5" s="61"/>
-      <c r="N5" s="60">
+      <c r="M5" s="67"/>
+      <c r="N5" s="66">
         <v>7</v>
       </c>
-      <c r="O5" s="61"/>
-      <c r="P5" s="60">
+      <c r="O5" s="67"/>
+      <c r="P5" s="66">
         <v>8</v>
       </c>
-      <c r="Q5" s="61"/>
-      <c r="R5" s="60">
+      <c r="Q5" s="67"/>
+      <c r="R5" s="66">
         <v>9</v>
       </c>
-      <c r="S5" s="61"/>
-      <c r="T5" s="60">
+      <c r="S5" s="67"/>
+      <c r="T5" s="66">
         <v>10</v>
       </c>
-      <c r="U5" s="61"/>
-      <c r="V5" s="60">
+      <c r="U5" s="67"/>
+      <c r="V5" s="66">
         <v>11</v>
       </c>
-      <c r="W5" s="61"/>
+      <c r="W5" s="67"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -1967,7 +2052,7 @@
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="49"/>
-      <c r="D7" s="80"/>
+      <c r="D7" s="64"/>
       <c r="E7" s="49"/>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -2076,7 +2161,7 @@
       <c r="B11" s="51"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
-      <c r="E11" s="34"/>
+      <c r="E11" s="56"/>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -2287,6 +2372,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Q3:W3"/>
     <mergeCell ref="A1:W1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="B3:E3"/>
@@ -2303,10 +2392,6 @@
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="F3:L3"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="Q3:W3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2316,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C78FCE7-630C-9647-8181-21056D9A31B5}">
   <dimension ref="A1:K214"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2329,12 +2414,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="62" t="s">
+      <c r="A1" s="68" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="62"/>
-      <c r="C1" s="62"/>
-      <c r="D1" s="62"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2392,7 +2477,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A6" s="72">
+      <c r="A6" s="80">
         <v>43592</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2406,7 +2491,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A7" s="73"/>
+      <c r="A7" s="81"/>
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
@@ -2418,7 +2503,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A8" s="73"/>
+      <c r="A8" s="81"/>
       <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
@@ -2430,7 +2515,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A9" s="73"/>
+      <c r="A9" s="81"/>
       <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
@@ -2442,7 +2527,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A10" s="73"/>
+      <c r="A10" s="81"/>
       <c r="B10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2454,7 +2539,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A11" s="73"/>
+      <c r="A11" s="81"/>
       <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2466,7 +2551,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A12" s="73"/>
+      <c r="A12" s="81"/>
       <c r="B12" s="11" t="s">
         <v>38</v>
       </c>
@@ -2478,7 +2563,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A13" s="73"/>
+      <c r="A13" s="81"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
@@ -2490,7 +2575,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A14" s="73"/>
+      <c r="A14" s="81"/>
       <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
@@ -2502,7 +2587,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A15" s="73"/>
+      <c r="A15" s="81"/>
       <c r="B15" s="11" t="s">
         <v>43</v>
       </c>
@@ -2514,7 +2599,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A16" s="74"/>
+      <c r="A16" s="82"/>
       <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
@@ -2524,15 +2609,15 @@
       <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A17" s="76" t="s">
+      <c r="A17" s="78" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="77"/>
-      <c r="C17" s="78">
+      <c r="B17" s="79"/>
+      <c r="C17" s="62">
         <f>SUM(C6:C16)</f>
         <v>0.32291666666666663</v>
       </c>
-      <c r="D17" s="75"/>
+      <c r="D17" s="61"/>
     </row>
     <row r="18" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
       <c r="A18" s="8">
@@ -2541,14 +2626,12 @@
       <c r="B18" s="11" t="s">
         <v>46</v>
       </c>
-      <c r="C18" s="9">
-        <v>6.25E-2</v>
-      </c>
-      <c r="D18" s="79"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="63"/>
     </row>
     <row r="19" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A19" s="8"/>
-      <c r="B19" s="81" t="s">
+      <c r="B19" s="65" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="9">
@@ -2558,17 +2641,17 @@
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A20" s="8"/>
-      <c r="B20" s="81" t="s">
+      <c r="B20" s="65" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="9">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A21" s="8"/>
-      <c r="B21" s="81" t="s">
+      <c r="B21" s="65" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="9">
@@ -2584,7 +2667,7 @@
         <v>52</v>
       </c>
       <c r="C22" s="9">
-        <v>4.1666666666666664E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="D22" s="14" t="s">
         <v>53</v>
@@ -2607,30 +2690,49 @@
       <c r="B24" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="9"/>
+      <c r="C24" s="9">
+        <v>8.3333333333333329E-2</v>
+      </c>
       <c r="D24" s="14" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A25" s="8"/>
-      <c r="B25" s="11"/>
-      <c r="C25" s="9"/>
-      <c r="D25" s="14"/>
-    </row>
-    <row r="26" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A26" s="8"/>
-      <c r="B26" s="11"/>
-      <c r="C26" s="9"/>
-      <c r="D26" s="14"/>
-    </row>
-    <row r="27" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A27" s="8"/>
-      <c r="B27" s="11"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="14"/>
-    </row>
-    <row r="28" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="B25" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D25" s="14" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A26" s="60"/>
+      <c r="B26" s="87" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="83">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D26" s="88" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A27" s="84" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="85"/>
+      <c r="C27" s="89">
+        <f>SUM(C19:C26)</f>
+        <v>0.32291666666666669</v>
+      </c>
+      <c r="D27" s="86"/>
+    </row>
+    <row r="28" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
       <c r="A28" s="8"/>
       <c r="B28" s="11"/>
       <c r="C28" s="9"/>
@@ -3753,10 +3855,11 @@
       <c r="D214" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="4">
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A6:A16"/>
+    <mergeCell ref="A27:B27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Bug camera - bcm2835-v4l2 et MMAL incompatible si actif en meme temps: https://www.raspberrypi.org/forums/viewtopic.php?t=232533
</commit_message>
<xml_diff>
--- a/Docs/EnzoRoy_Planning_Taches.xlsx
+++ b/Docs/EnzoRoy_Planning_Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoroy/Desktop/EnzoRoy_TPI/BotCleaner/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A1C7F08-A316-8F4B-B524-5E30809A089B}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE2DDB3-0835-FF44-9915-015E1A3B5EEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" activeTab="2" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
   <si>
     <t>Date</t>
   </si>
@@ -222,6 +222,75 @@
   </si>
   <si>
     <t>Total J2</t>
+  </si>
+  <si>
+    <t>Résolution d'erreur requête POST</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gestion des requêtes post </t>
+  </si>
+  <si>
+    <t>function ne retournait aucune réponse: code 200 à retourner lorsque tout ce passe bien</t>
+  </si>
+  <si>
+    <t>visite expert</t>
+  </si>
+  <si>
+    <t xml:space="preserve">présation de l'avancée du TPI, aucunes questions spécifiques, </t>
+  </si>
+  <si>
+    <t>class robot</t>
+  </si>
+  <si>
+    <t>remise au propre class robot de waveshare</t>
+  </si>
+  <si>
+    <t>mise au propre code pour intégrer la class robot</t>
+  </si>
+  <si>
+    <t>ajout de la camera dans la classe robot</t>
+  </si>
+  <si>
+    <t>Création des classes</t>
+  </si>
+  <si>
+    <t>mise au propre, POO</t>
+  </si>
+  <si>
+    <t>class controller</t>
+  </si>
+  <si>
+    <t>Controler alpha bot depuis manette web</t>
+  </si>
+  <si>
+    <t>camera dans la classe robot mais stream resté dans le main</t>
+  </si>
+  <si>
+    <t>class motor</t>
+  </si>
+  <si>
+    <t>recherche des pin moteurs et cleanup a partir code de waveshare</t>
+  </si>
+  <si>
+    <t>lien entre main et alphabot</t>
+  </si>
+  <si>
+    <t>Total J3</t>
+  </si>
+  <si>
+    <t>problemes de post resolu</t>
+  </si>
+  <si>
+    <t>résolution erreur picamera</t>
+  </si>
+  <si>
+    <t>camera déjà utilisé ? Mémoire insuffisante ? : picamera.exc.PiCameraMMALError: Failed to enable connection: Out of resources</t>
+  </si>
+  <si>
+    <t>bug GPIO, cam…</t>
+  </si>
+  <si>
+    <t>reset de l'OS</t>
   </si>
 </sst>
 </file>
@@ -250,7 +319,7 @@
       <name val="Helvetica Neue Moyen"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -293,6 +362,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF2E5496"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="35">
     <border>
@@ -642,7 +717,7 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom style="medium">
+      <bottom style="double">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -652,10 +727,10 @@
         <color indexed="64"/>
       </left>
       <right/>
-      <top style="medium">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -665,10 +740,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -680,10 +755,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top style="medium">
+      <top style="double">
         <color indexed="64"/>
       </top>
-      <bottom style="double">
+      <bottom style="thick">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -692,8 +767,25 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right/>
-      <top/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thick">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color indexed="64"/>
+      </top>
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
@@ -703,22 +795,11 @@
       <left style="thin">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
       <right/>
-      <top/>
-      <bottom style="double">
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -728,8 +809,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="double">
+      <top style="double">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -843,15 +926,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="19" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="17" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="23" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -859,41 +933,72 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="3"/>
     </xf>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="30" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="20" fontId="0" fillId="7" borderId="33" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="28" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -904,39 +1009,18 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="0" fillId="7" borderId="32" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF2E5496"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1247,8 +1331,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247B9052-0D38-E749-9EA6-411F034D0277}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1258,145 +1342,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="70" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="72">
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="73">
         <v>43592</v>
       </c>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="74"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="75" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="76" t="s">
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="78"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="66">
+      <c r="B5" s="79">
         <v>1</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="66">
+      <c r="C5" s="80"/>
+      <c r="D5" s="79">
         <v>2</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="66">
+      <c r="E5" s="80"/>
+      <c r="F5" s="79">
         <v>3</v>
       </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="66">
+      <c r="G5" s="80"/>
+      <c r="H5" s="79">
         <v>4</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="66">
+      <c r="I5" s="80"/>
+      <c r="J5" s="79">
         <v>5</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="66">
+      <c r="K5" s="80"/>
+      <c r="L5" s="79">
         <v>6</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="66">
+      <c r="M5" s="80"/>
+      <c r="N5" s="79">
         <v>7</v>
       </c>
-      <c r="O5" s="67"/>
-      <c r="P5" s="66">
+      <c r="O5" s="80"/>
+      <c r="P5" s="79">
         <v>8</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="66">
+      <c r="Q5" s="80"/>
+      <c r="R5" s="79">
         <v>9</v>
       </c>
-      <c r="S5" s="67"/>
-      <c r="T5" s="66">
+      <c r="S5" s="80"/>
+      <c r="T5" s="79">
         <v>10</v>
       </c>
-      <c r="U5" s="67"/>
-      <c r="V5" s="66">
+      <c r="U5" s="80"/>
+      <c r="V5" s="79">
         <v>11</v>
       </c>
-      <c r="W5" s="67"/>
+      <c r="W5" s="80"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -1592,8 +1676,8 @@
       <c r="J11" s="33"/>
       <c r="K11" s="33"/>
       <c r="L11" s="33"/>
-      <c r="M11" s="33"/>
-      <c r="N11" s="33"/>
+      <c r="M11" s="34"/>
+      <c r="N11" s="34"/>
       <c r="O11" s="3"/>
       <c r="P11" s="3"/>
       <c r="Q11" s="3"/>
@@ -1619,8 +1703,8 @@
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
       <c r="L12" s="3"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="3"/>
+      <c r="M12" s="66"/>
+      <c r="N12" s="66"/>
       <c r="O12" s="33"/>
       <c r="P12" s="33"/>
       <c r="Q12" s="3"/>
@@ -1710,7 +1794,7 @@
       <c r="T15" s="33"/>
       <c r="U15" s="33"/>
       <c r="V15" s="33"/>
-      <c r="W15" s="36"/>
+      <c r="W15" s="89"/>
     </row>
     <row r="16" spans="1:23" ht="35" customHeight="1">
       <c r="A16" s="47" t="s">
@@ -1795,6 +1879,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F3:L3"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="F5:G5"/>
+    <mergeCell ref="H5:I5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="N5:O5"/>
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
@@ -1805,16 +1899,6 @@
     <mergeCell ref="F2:L2"/>
     <mergeCell ref="M2:P2"/>
     <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F3:L3"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="F5:G5"/>
-    <mergeCell ref="H5:I5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="N5:O5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1822,10 +1906,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779F402-4327-4345-BFB9-00C0C178FF50}">
-  <dimension ref="A1:W18"/>
+  <dimension ref="A1:W19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1835,145 +1919,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
-      <c r="E1" s="68"/>
-      <c r="F1" s="68"/>
-      <c r="G1" s="68"/>
-      <c r="H1" s="68"/>
-      <c r="I1" s="68"/>
-      <c r="J1" s="68"/>
-      <c r="K1" s="68"/>
-      <c r="L1" s="68"/>
-      <c r="M1" s="68"/>
-      <c r="N1" s="68"/>
-      <c r="O1" s="68"/>
-      <c r="P1" s="68"/>
-      <c r="Q1" s="68"/>
-      <c r="R1" s="68"/>
-      <c r="S1" s="68"/>
-      <c r="T1" s="68"/>
-      <c r="U1" s="68"/>
-      <c r="V1" s="68"/>
-      <c r="W1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
+      <c r="E1" s="69"/>
+      <c r="F1" s="69"/>
+      <c r="G1" s="69"/>
+      <c r="H1" s="69"/>
+      <c r="I1" s="69"/>
+      <c r="J1" s="69"/>
+      <c r="K1" s="69"/>
+      <c r="L1" s="69"/>
+      <c r="M1" s="69"/>
+      <c r="N1" s="69"/>
+      <c r="O1" s="69"/>
+      <c r="P1" s="69"/>
+      <c r="Q1" s="69"/>
+      <c r="R1" s="69"/>
+      <c r="S1" s="69"/>
+      <c r="T1" s="69"/>
+      <c r="U1" s="69"/>
+      <c r="V1" s="69"/>
+      <c r="W1" s="69"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="70" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="71" t="s">
+      <c r="C2" s="71"/>
+      <c r="D2" s="71"/>
+      <c r="E2" s="71"/>
+      <c r="F2" s="72" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="71"/>
-      <c r="H2" s="71"/>
-      <c r="I2" s="71"/>
-      <c r="J2" s="71"/>
-      <c r="K2" s="71"/>
-      <c r="L2" s="71"/>
-      <c r="M2" s="70" t="s">
+      <c r="G2" s="72"/>
+      <c r="H2" s="72"/>
+      <c r="I2" s="72"/>
+      <c r="J2" s="72"/>
+      <c r="K2" s="72"/>
+      <c r="L2" s="72"/>
+      <c r="M2" s="71" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="70"/>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="72">
+      <c r="N2" s="71"/>
+      <c r="O2" s="71"/>
+      <c r="P2" s="71"/>
+      <c r="Q2" s="73">
         <v>43592</v>
       </c>
-      <c r="R2" s="72"/>
-      <c r="S2" s="72"/>
-      <c r="T2" s="72"/>
-      <c r="U2" s="72"/>
-      <c r="V2" s="72"/>
-      <c r="W2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="74"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="74" t="s">
+      <c r="B3" s="75" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="75"/>
-      <c r="D3" s="75"/>
-      <c r="E3" s="75"/>
-      <c r="F3" s="76" t="s">
+      <c r="C3" s="76"/>
+      <c r="D3" s="76"/>
+      <c r="E3" s="76"/>
+      <c r="F3" s="77" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="76"/>
-      <c r="H3" s="76"/>
-      <c r="I3" s="76"/>
-      <c r="J3" s="76"/>
-      <c r="K3" s="76"/>
-      <c r="L3" s="76"/>
-      <c r="M3" s="75" t="s">
+      <c r="G3" s="77"/>
+      <c r="H3" s="77"/>
+      <c r="I3" s="77"/>
+      <c r="J3" s="77"/>
+      <c r="K3" s="77"/>
+      <c r="L3" s="77"/>
+      <c r="M3" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="75"/>
-      <c r="O3" s="75"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="76" t="s">
+      <c r="N3" s="76"/>
+      <c r="O3" s="76"/>
+      <c r="P3" s="76"/>
+      <c r="Q3" s="77" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="76"/>
-      <c r="S3" s="76"/>
-      <c r="T3" s="76"/>
-      <c r="U3" s="76"/>
-      <c r="V3" s="76"/>
-      <c r="W3" s="77"/>
+      <c r="R3" s="77"/>
+      <c r="S3" s="77"/>
+      <c r="T3" s="77"/>
+      <c r="U3" s="77"/>
+      <c r="V3" s="77"/>
+      <c r="W3" s="78"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="66">
+      <c r="B5" s="79">
         <v>1</v>
       </c>
-      <c r="C5" s="67"/>
-      <c r="D5" s="66">
+      <c r="C5" s="80"/>
+      <c r="D5" s="79">
         <v>2</v>
       </c>
-      <c r="E5" s="67"/>
-      <c r="F5" s="66">
+      <c r="E5" s="80"/>
+      <c r="F5" s="79">
         <v>3</v>
       </c>
-      <c r="G5" s="67"/>
-      <c r="H5" s="66">
+      <c r="G5" s="80"/>
+      <c r="H5" s="79">
         <v>4</v>
       </c>
-      <c r="I5" s="67"/>
-      <c r="J5" s="66">
+      <c r="I5" s="80"/>
+      <c r="J5" s="79">
         <v>5</v>
       </c>
-      <c r="K5" s="67"/>
-      <c r="L5" s="66">
+      <c r="K5" s="80"/>
+      <c r="L5" s="79">
         <v>6</v>
       </c>
-      <c r="M5" s="67"/>
-      <c r="N5" s="66">
+      <c r="M5" s="80"/>
+      <c r="N5" s="79">
         <v>7</v>
       </c>
-      <c r="O5" s="67"/>
-      <c r="P5" s="66">
+      <c r="O5" s="80"/>
+      <c r="P5" s="79">
         <v>8</v>
       </c>
-      <c r="Q5" s="67"/>
-      <c r="R5" s="66">
+      <c r="Q5" s="80"/>
+      <c r="R5" s="79">
         <v>9</v>
       </c>
-      <c r="S5" s="67"/>
-      <c r="T5" s="66">
+      <c r="S5" s="80"/>
+      <c r="T5" s="79">
         <v>10</v>
       </c>
-      <c r="U5" s="67"/>
-      <c r="V5" s="66">
+      <c r="U5" s="80"/>
+      <c r="V5" s="79">
         <v>11</v>
       </c>
-      <c r="W5" s="67"/>
+      <c r="W5" s="80"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -2052,7 +2136,7 @@
       </c>
       <c r="B7" s="55"/>
       <c r="C7" s="49"/>
-      <c r="D7" s="64"/>
+      <c r="D7" s="61"/>
       <c r="E7" s="49"/>
       <c r="F7" s="49"/>
       <c r="G7" s="49"/>
@@ -2083,7 +2167,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
+      <c r="H8" s="56"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
@@ -2110,7 +2194,7 @@
       <c r="E9" s="56"/>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
-      <c r="H9" s="34"/>
+      <c r="H9" s="56"/>
       <c r="I9" s="34"/>
       <c r="J9" s="34"/>
       <c r="K9" s="34"/>
@@ -2129,14 +2213,14 @@
     </row>
     <row r="10" spans="1:23" ht="35" customHeight="1">
       <c r="A10" s="47" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="B10" s="51"/>
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
       <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
+      <c r="G10" s="56"/>
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
       <c r="J10" s="34"/>
@@ -2156,12 +2240,12 @@
     </row>
     <row r="11" spans="1:23" ht="35" customHeight="1">
       <c r="A11" s="47" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B11" s="51"/>
       <c r="C11" s="34"/>
       <c r="D11" s="34"/>
-      <c r="E11" s="56"/>
+      <c r="E11" s="34"/>
       <c r="F11" s="34"/>
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
@@ -2183,14 +2267,14 @@
     </row>
     <row r="12" spans="1:23" ht="35" customHeight="1">
       <c r="A12" s="47" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="51"/>
       <c r="C12" s="34"/>
       <c r="D12" s="34"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="34"/>
-      <c r="G12" s="34"/>
+      <c r="E12" s="56"/>
+      <c r="F12" s="56"/>
+      <c r="G12" s="56"/>
       <c r="H12" s="34"/>
       <c r="I12" s="34"/>
       <c r="J12" s="34"/>
@@ -2210,7 +2294,7 @@
     </row>
     <row r="13" spans="1:23" ht="35" customHeight="1">
       <c r="A13" s="47" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
       <c r="B13" s="51"/>
       <c r="C13" s="34"/>
@@ -2237,7 +2321,7 @@
     </row>
     <row r="14" spans="1:23" ht="35" customHeight="1">
       <c r="A14" s="47" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="34"/>
@@ -2264,12 +2348,12 @@
     </row>
     <row r="15" spans="1:23" ht="35" customHeight="1">
       <c r="A15" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="56"/>
-      <c r="D15" s="56"/>
-      <c r="E15" s="56"/>
+        <v>16</v>
+      </c>
+      <c r="B15" s="51"/>
+      <c r="C15" s="34"/>
+      <c r="D15" s="34"/>
+      <c r="E15" s="34"/>
       <c r="F15" s="34"/>
       <c r="G15" s="34"/>
       <c r="H15" s="34"/>
@@ -2291,16 +2375,16 @@
     </row>
     <row r="16" spans="1:23" ht="35" customHeight="1">
       <c r="A16" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="51"/>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+        <v>17</v>
+      </c>
+      <c r="B16" s="58"/>
+      <c r="C16" s="56"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="34"/>
-      <c r="H16" s="34"/>
-      <c r="I16" s="34"/>
+      <c r="H16" s="56"/>
+      <c r="I16" s="56"/>
       <c r="J16" s="34"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
@@ -2318,7 +2402,7 @@
     </row>
     <row r="17" spans="1:23" ht="35" customHeight="1">
       <c r="A17" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B17" s="51"/>
       <c r="C17" s="34"/>
@@ -2343,43 +2427,62 @@
       <c r="V17" s="34"/>
       <c r="W17" s="52"/>
     </row>
-    <row r="18" spans="1:23" ht="35" customHeight="1" thickBot="1">
-      <c r="A18" s="48" t="s">
+    <row r="18" spans="1:23" ht="35" customHeight="1">
+      <c r="A18" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="51"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+      <c r="G18" s="34"/>
+      <c r="H18" s="34"/>
+      <c r="I18" s="34"/>
+      <c r="J18" s="34"/>
+      <c r="K18" s="34"/>
+      <c r="L18" s="34"/>
+      <c r="M18" s="34"/>
+      <c r="N18" s="34"/>
+      <c r="O18" s="34"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="34"/>
+      <c r="R18" s="34"/>
+      <c r="S18" s="34"/>
+      <c r="T18" s="34"/>
+      <c r="U18" s="34"/>
+      <c r="V18" s="34"/>
+      <c r="W18" s="52"/>
+    </row>
+    <row r="19" spans="1:23" ht="35" customHeight="1" thickBot="1">
+      <c r="A19" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B18" s="59"/>
-      <c r="C18" s="57"/>
-      <c r="D18" s="57"/>
-      <c r="E18" s="57"/>
-      <c r="F18" s="53"/>
-      <c r="G18" s="53"/>
-      <c r="H18" s="53"/>
-      <c r="I18" s="53"/>
-      <c r="J18" s="53"/>
-      <c r="K18" s="53"/>
-      <c r="L18" s="53"/>
-      <c r="M18" s="53"/>
-      <c r="N18" s="53"/>
-      <c r="O18" s="53"/>
-      <c r="P18" s="53"/>
-      <c r="Q18" s="53"/>
-      <c r="R18" s="53"/>
-      <c r="S18" s="53"/>
-      <c r="T18" s="53"/>
-      <c r="U18" s="53"/>
-      <c r="V18" s="53"/>
-      <c r="W18" s="54"/>
+      <c r="B19" s="59"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="57"/>
+      <c r="F19" s="57"/>
+      <c r="G19" s="57"/>
+      <c r="H19" s="57"/>
+      <c r="I19" s="57"/>
+      <c r="J19" s="53"/>
+      <c r="K19" s="53"/>
+      <c r="L19" s="53"/>
+      <c r="M19" s="53"/>
+      <c r="N19" s="53"/>
+      <c r="O19" s="53"/>
+      <c r="P19" s="53"/>
+      <c r="Q19" s="53"/>
+      <c r="R19" s="53"/>
+      <c r="S19" s="53"/>
+      <c r="T19" s="53"/>
+      <c r="U19" s="53"/>
+      <c r="V19" s="53"/>
+      <c r="W19" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F2:L2"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
@@ -2391,6 +2494,14 @@
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F2:L2"/>
     <mergeCell ref="F3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2401,8 +2512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C78FCE7-630C-9647-8181-21056D9A31B5}">
   <dimension ref="A1:K214"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D39" sqref="D39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2414,12 +2525,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="69" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="68"/>
-      <c r="C1" s="68"/>
-      <c r="D1" s="68"/>
+      <c r="B1" s="69"/>
+      <c r="C1" s="69"/>
+      <c r="D1" s="69"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2477,7 +2588,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A6" s="80">
+      <c r="A6" s="88">
         <v>43592</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2491,7 +2602,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A7" s="81"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
@@ -2503,7 +2614,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A8" s="81"/>
+      <c r="A8" s="84"/>
       <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
@@ -2515,7 +2626,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A9" s="81"/>
+      <c r="A9" s="84"/>
       <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
@@ -2527,7 +2638,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A10" s="81"/>
+      <c r="A10" s="84"/>
       <c r="B10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2539,7 +2650,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A11" s="81"/>
+      <c r="A11" s="84"/>
       <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2551,7 +2662,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A12" s="81"/>
+      <c r="A12" s="84"/>
       <c r="B12" s="11" t="s">
         <v>38</v>
       </c>
@@ -2563,7 +2674,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A13" s="81"/>
+      <c r="A13" s="84"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
@@ -2575,7 +2686,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A14" s="81"/>
+      <c r="A14" s="84"/>
       <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
@@ -2587,7 +2698,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A15" s="81"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="11" t="s">
         <v>43</v>
       </c>
@@ -2599,7 +2710,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A16" s="82"/>
+      <c r="A16" s="84"/>
       <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
@@ -2608,30 +2719,30 @@
       </c>
       <c r="D16" s="14"/>
     </row>
-    <row r="17" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A17" s="78" t="s">
+    <row r="17" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A17" s="86" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="79"/>
-      <c r="C17" s="62">
+      <c r="B17" s="87"/>
+      <c r="C17" s="63">
         <f>SUM(C6:C16)</f>
         <v>0.32291666666666663</v>
       </c>
-      <c r="D17" s="61"/>
+      <c r="D17" s="64"/>
     </row>
     <row r="18" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
-      <c r="A18" s="8">
+      <c r="A18" s="83">
         <v>43593</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>46</v>
       </c>
       <c r="C18" s="9"/>
-      <c r="D18" s="63"/>
+      <c r="D18" s="60"/>
     </row>
     <row r="19" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A19" s="8"/>
-      <c r="B19" s="65" t="s">
+      <c r="A19" s="84"/>
+      <c r="B19" s="62" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="9">
@@ -2640,8 +2751,8 @@
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A20" s="8"/>
-      <c r="B20" s="65" t="s">
+      <c r="A20" s="84"/>
+      <c r="B20" s="62" t="s">
         <v>49</v>
       </c>
       <c r="C20" s="9">
@@ -2650,8 +2761,8 @@
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A21" s="8"/>
-      <c r="B21" s="65" t="s">
+      <c r="A21" s="84"/>
+      <c r="B21" s="62" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="9">
@@ -2662,7 +2773,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A22" s="8"/>
+      <c r="A22" s="84"/>
       <c r="B22" s="11" t="s">
         <v>52</v>
       </c>
@@ -2674,7 +2785,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A23" s="8"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="11" t="s">
         <v>54</v>
       </c>
@@ -2686,7 +2797,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A24" s="8"/>
+      <c r="A24" s="84"/>
       <c r="B24" s="11" t="s">
         <v>56</v>
       </c>
@@ -2698,7 +2809,7 @@
       </c>
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A25" s="8"/>
+      <c r="A25" s="84"/>
       <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
@@ -2710,99 +2821,170 @@
       </c>
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A26" s="60"/>
-      <c r="B26" s="87" t="s">
+      <c r="A26" s="85"/>
+      <c r="B26" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C26" s="83">
+      <c r="C26" s="9">
         <v>4.1666666666666664E-2</v>
       </c>
-      <c r="D26" s="88" t="s">
+      <c r="D26" s="14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A27" s="84" t="s">
+    <row r="27" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A27" s="86" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="85"/>
-      <c r="C27" s="89">
+      <c r="B27" s="87"/>
+      <c r="C27" s="63">
         <f>SUM(C19:C26)</f>
         <v>0.32291666666666669</v>
       </c>
-      <c r="D27" s="86"/>
+      <c r="D27" s="65"/>
     </row>
     <row r="28" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
-      <c r="A28" s="8"/>
-      <c r="B28" s="11"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="14"/>
+      <c r="A28" s="83">
+        <v>43594</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D28" s="14" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="29" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A29" s="8"/>
-      <c r="B29" s="11"/>
-      <c r="C29" s="9"/>
-      <c r="D29" s="14"/>
+      <c r="A29" s="84"/>
+      <c r="B29" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="C29" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D29" s="14" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="30" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A30" s="8"/>
-      <c r="B30" s="11"/>
-      <c r="C30" s="9"/>
-      <c r="D30" s="14"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C30" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D30" s="14" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="31" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A31" s="8"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="14"/>
+      <c r="A31" s="84"/>
+      <c r="B31" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C31" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D31" s="14" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="32" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A32" s="8"/>
-      <c r="B32" s="11"/>
-      <c r="C32" s="9"/>
-      <c r="D32" s="14"/>
+      <c r="A32" s="84"/>
+      <c r="B32" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D32" s="14" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="33" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A33" s="8"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="9"/>
-      <c r="D33" s="14"/>
+      <c r="A33" s="84"/>
+      <c r="B33" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="34" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A34" s="8"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="14"/>
+      <c r="A34" s="84"/>
+      <c r="B34" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C34" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D34" s="14" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="35" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A35" s="8"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="9"/>
-      <c r="D35" s="14"/>
-    </row>
-    <row r="36" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A36" s="8"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="9"/>
-      <c r="D36" s="14"/>
-    </row>
-    <row r="37" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A37" s="8"/>
-      <c r="B37" s="11"/>
-      <c r="C37" s="9"/>
-      <c r="D37" s="14"/>
+      <c r="A35" s="84"/>
+      <c r="B35" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C35" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D35" s="14" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A36" s="85"/>
+      <c r="B36" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C36" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D36" s="14" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A37" s="81" t="s">
+        <v>80</v>
+      </c>
+      <c r="B37" s="82"/>
+      <c r="C37" s="67">
+        <f>SUM(C28:C36)</f>
+        <v>0.3125</v>
+      </c>
+      <c r="D37" s="68"/>
     </row>
     <row r="38" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A38" s="8"/>
-      <c r="B38" s="11"/>
+      <c r="A38" s="8">
+        <v>43598</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>82</v>
+      </c>
       <c r="C38" s="9"/>
-      <c r="D38" s="14"/>
+      <c r="D38" s="14" t="s">
+        <v>83</v>
+      </c>
     </row>
     <row r="39" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A39" s="8"/>
-      <c r="B39" s="11"/>
+      <c r="B39" s="11" t="s">
+        <v>84</v>
+      </c>
       <c r="C39" s="9"/>
-      <c r="D39" s="14"/>
+      <c r="D39" s="14" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="40" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A40" s="8"/>
@@ -3855,11 +4037,14 @@
       <c r="D214" s="14"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="A37:B37"/>
+    <mergeCell ref="A28:A36"/>
     <mergeCell ref="A1:D1"/>
     <mergeCell ref="A17:B17"/>
     <mergeCell ref="A6:A16"/>
     <mergeCell ref="A27:B27"/>
+    <mergeCell ref="A18:A26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Recuperation image du flux pour analyse
</commit_message>
<xml_diff>
--- a/Docs/EnzoRoy_Planning_Taches.xlsx
+++ b/Docs/EnzoRoy_Planning_Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoroy/Desktop/EnzoRoy_TPI/BotCleaner/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE2DDB3-0835-FF44-9915-015E1A3B5EEB}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4ABBF5D9-2C5B-1349-9FBE-2370FF65039C}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="18880" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="33600" windowHeight="21000" activeTab="1" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="114">
   <si>
     <t>Date</t>
   </si>
@@ -291,6 +291,90 @@
   </si>
   <si>
     <t>reset de l'OS</t>
+  </si>
+  <si>
+    <t>Finalisation</t>
+  </si>
+  <si>
+    <t>Correction bug</t>
+  </si>
+  <si>
+    <t>aide de Mr. Bonvin</t>
+  </si>
+  <si>
+    <t>erreur persiste</t>
+  </si>
+  <si>
+    <t>nettoyage du code</t>
+  </si>
+  <si>
+    <t>afin de facilite le recherche sur l origine de l erreur</t>
+  </si>
+  <si>
+    <t>je ne comprennais pas l'origine du bug puisque aucun script n'était censé etre actif</t>
+  </si>
+  <si>
+    <t>resolution du bug</t>
+  </si>
+  <si>
+    <t>parametrage de pycharm et remise en place de la dernière version</t>
+  </si>
+  <si>
+    <t>recherche forum sur code d'erreur</t>
+  </si>
+  <si>
+    <t xml:space="preserve">picamera: out of memory / V4l2 et MMAL </t>
+  </si>
+  <si>
+    <t>Total J4</t>
+  </si>
+  <si>
+    <t>doc</t>
+  </si>
+  <si>
+    <t>tests</t>
+  </si>
+  <si>
+    <t>vérifier que le problème ne persiste plus et que tout refonctionne correctement</t>
+  </si>
+  <si>
+    <t>raison du bug</t>
+  </si>
+  <si>
+    <t>regrouper code</t>
+  </si>
+  <si>
+    <t>cv2 recupération flux video</t>
+  </si>
+  <si>
+    <t>trop de reprise de code, peu de compréhension… trouver une autre solution</t>
+  </si>
+  <si>
+    <t>remettre code au "propre"</t>
+  </si>
+  <si>
+    <t>flask envoie derniere frame</t>
+  </si>
+  <si>
+    <t>recuperation de la derniere frame</t>
+  </si>
+  <si>
+    <t>analyse image</t>
+  </si>
+  <si>
+    <t>nouvelle app route avec response de output.frame</t>
+  </si>
+  <si>
+    <t>utilisation de PIL et de requests</t>
+  </si>
+  <si>
+    <t>skimage io propose imread bien plus lisible que précédemment</t>
+  </si>
+  <si>
+    <t>cv2 - scikit : quelques tests</t>
+  </si>
+  <si>
+    <t>Total J5</t>
   </si>
 </sst>
 </file>
@@ -821,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="90">
+  <cellXfs count="91">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -949,6 +1033,24 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -967,24 +1069,6 @@
     <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1009,7 +1093,10 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="18" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1331,8 +1418,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{247B9052-0D38-E749-9EA6-411F034D0277}">
   <dimension ref="A1:W18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1342,145 +1429,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="71" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="73">
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="79">
         <v>43592</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="74"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="80"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="77" t="s">
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="76" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="77" t="s">
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="78"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="72"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="73">
         <v>1</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="79">
+      <c r="C5" s="74"/>
+      <c r="D5" s="73">
         <v>2</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79">
+      <c r="E5" s="74"/>
+      <c r="F5" s="73">
         <v>3</v>
       </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="79">
+      <c r="G5" s="74"/>
+      <c r="H5" s="73">
         <v>4</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="79">
+      <c r="I5" s="74"/>
+      <c r="J5" s="73">
         <v>5</v>
       </c>
-      <c r="K5" s="80"/>
-      <c r="L5" s="79">
+      <c r="K5" s="74"/>
+      <c r="L5" s="73">
         <v>6</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="79">
+      <c r="M5" s="74"/>
+      <c r="N5" s="73">
         <v>7</v>
       </c>
-      <c r="O5" s="80"/>
-      <c r="P5" s="79">
+      <c r="O5" s="74"/>
+      <c r="P5" s="73">
         <v>8</v>
       </c>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="79">
+      <c r="Q5" s="74"/>
+      <c r="R5" s="73">
         <v>9</v>
       </c>
-      <c r="S5" s="80"/>
-      <c r="T5" s="79">
+      <c r="S5" s="74"/>
+      <c r="T5" s="73">
         <v>10</v>
       </c>
-      <c r="U5" s="80"/>
-      <c r="V5" s="79">
+      <c r="U5" s="74"/>
+      <c r="V5" s="73">
         <v>11</v>
       </c>
-      <c r="W5" s="80"/>
+      <c r="W5" s="74"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -1794,7 +1881,7 @@
       <c r="T15" s="33"/>
       <c r="U15" s="33"/>
       <c r="V15" s="33"/>
-      <c r="W15" s="89"/>
+      <c r="W15" s="52"/>
     </row>
     <row r="16" spans="1:23" ht="35" customHeight="1">
       <c r="A16" s="47" t="s">
@@ -1878,7 +1965,13 @@
       <c r="W18" s="40"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:L3"/>
     <mergeCell ref="M3:P3"/>
@@ -1894,11 +1987,6 @@
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="L5:M5"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1906,10 +1994,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779F402-4327-4345-BFB9-00C0C178FF50}">
-  <dimension ref="A1:W19"/>
+  <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -1919,145 +2007,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
-      <c r="E1" s="69"/>
-      <c r="F1" s="69"/>
-      <c r="G1" s="69"/>
-      <c r="H1" s="69"/>
-      <c r="I1" s="69"/>
-      <c r="J1" s="69"/>
-      <c r="K1" s="69"/>
-      <c r="L1" s="69"/>
-      <c r="M1" s="69"/>
-      <c r="N1" s="69"/>
-      <c r="O1" s="69"/>
-      <c r="P1" s="69"/>
-      <c r="Q1" s="69"/>
-      <c r="R1" s="69"/>
-      <c r="S1" s="69"/>
-      <c r="T1" s="69"/>
-      <c r="U1" s="69"/>
-      <c r="V1" s="69"/>
-      <c r="W1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
+      <c r="E1" s="75"/>
+      <c r="F1" s="75"/>
+      <c r="G1" s="75"/>
+      <c r="H1" s="75"/>
+      <c r="I1" s="75"/>
+      <c r="J1" s="75"/>
+      <c r="K1" s="75"/>
+      <c r="L1" s="75"/>
+      <c r="M1" s="75"/>
+      <c r="N1" s="75"/>
+      <c r="O1" s="75"/>
+      <c r="P1" s="75"/>
+      <c r="Q1" s="75"/>
+      <c r="R1" s="75"/>
+      <c r="S1" s="75"/>
+      <c r="T1" s="75"/>
+      <c r="U1" s="75"/>
+      <c r="V1" s="75"/>
+      <c r="W1" s="75"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="76" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="71"/>
-      <c r="D2" s="71"/>
-      <c r="E2" s="71"/>
-      <c r="F2" s="72" t="s">
+      <c r="C2" s="77"/>
+      <c r="D2" s="77"/>
+      <c r="E2" s="77"/>
+      <c r="F2" s="78" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="72"/>
-      <c r="H2" s="72"/>
-      <c r="I2" s="72"/>
-      <c r="J2" s="72"/>
-      <c r="K2" s="72"/>
-      <c r="L2" s="72"/>
-      <c r="M2" s="71" t="s">
+      <c r="G2" s="78"/>
+      <c r="H2" s="78"/>
+      <c r="I2" s="78"/>
+      <c r="J2" s="78"/>
+      <c r="K2" s="78"/>
+      <c r="L2" s="78"/>
+      <c r="M2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="71"/>
-      <c r="O2" s="71"/>
-      <c r="P2" s="71"/>
-      <c r="Q2" s="73">
+      <c r="N2" s="77"/>
+      <c r="O2" s="77"/>
+      <c r="P2" s="77"/>
+      <c r="Q2" s="79">
         <v>43592</v>
       </c>
-      <c r="R2" s="73"/>
-      <c r="S2" s="73"/>
-      <c r="T2" s="73"/>
-      <c r="U2" s="73"/>
-      <c r="V2" s="73"/>
-      <c r="W2" s="74"/>
+      <c r="R2" s="79"/>
+      <c r="S2" s="79"/>
+      <c r="T2" s="79"/>
+      <c r="U2" s="79"/>
+      <c r="V2" s="79"/>
+      <c r="W2" s="80"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="75" t="s">
+      <c r="B3" s="69" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="76"/>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76"/>
-      <c r="F3" s="77" t="s">
+      <c r="C3" s="70"/>
+      <c r="D3" s="70"/>
+      <c r="E3" s="70"/>
+      <c r="F3" s="71" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="77"/>
-      <c r="H3" s="77"/>
-      <c r="I3" s="77"/>
-      <c r="J3" s="77"/>
-      <c r="K3" s="77"/>
-      <c r="L3" s="77"/>
-      <c r="M3" s="76" t="s">
+      <c r="G3" s="71"/>
+      <c r="H3" s="71"/>
+      <c r="I3" s="71"/>
+      <c r="J3" s="71"/>
+      <c r="K3" s="71"/>
+      <c r="L3" s="71"/>
+      <c r="M3" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="76"/>
-      <c r="O3" s="76"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="77" t="s">
+      <c r="N3" s="70"/>
+      <c r="O3" s="70"/>
+      <c r="P3" s="70"/>
+      <c r="Q3" s="71" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="77"/>
-      <c r="S3" s="77"/>
-      <c r="T3" s="77"/>
-      <c r="U3" s="77"/>
-      <c r="V3" s="77"/>
-      <c r="W3" s="78"/>
+      <c r="R3" s="71"/>
+      <c r="S3" s="71"/>
+      <c r="T3" s="71"/>
+      <c r="U3" s="71"/>
+      <c r="V3" s="71"/>
+      <c r="W3" s="72"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="79">
+      <c r="B5" s="73">
         <v>1</v>
       </c>
-      <c r="C5" s="80"/>
-      <c r="D5" s="79">
+      <c r="C5" s="74"/>
+      <c r="D5" s="73">
         <v>2</v>
       </c>
-      <c r="E5" s="80"/>
-      <c r="F5" s="79">
+      <c r="E5" s="74"/>
+      <c r="F5" s="73">
         <v>3</v>
       </c>
-      <c r="G5" s="80"/>
-      <c r="H5" s="79">
+      <c r="G5" s="74"/>
+      <c r="H5" s="73">
         <v>4</v>
       </c>
-      <c r="I5" s="80"/>
-      <c r="J5" s="79">
+      <c r="I5" s="74"/>
+      <c r="J5" s="73">
         <v>5</v>
       </c>
-      <c r="K5" s="80"/>
-      <c r="L5" s="79">
+      <c r="K5" s="74"/>
+      <c r="L5" s="73">
         <v>6</v>
       </c>
-      <c r="M5" s="80"/>
-      <c r="N5" s="79">
+      <c r="M5" s="74"/>
+      <c r="N5" s="73">
         <v>7</v>
       </c>
-      <c r="O5" s="80"/>
-      <c r="P5" s="79">
+      <c r="O5" s="74"/>
+      <c r="P5" s="73">
         <v>8</v>
       </c>
-      <c r="Q5" s="80"/>
-      <c r="R5" s="79">
+      <c r="Q5" s="74"/>
+      <c r="R5" s="73">
         <v>9</v>
       </c>
-      <c r="S5" s="80"/>
-      <c r="T5" s="79">
+      <c r="S5" s="74"/>
+      <c r="T5" s="73">
         <v>10</v>
       </c>
-      <c r="U5" s="80"/>
-      <c r="V5" s="79">
+      <c r="U5" s="74"/>
+      <c r="V5" s="73">
         <v>11</v>
       </c>
-      <c r="W5" s="80"/>
+      <c r="W5" s="74"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -2167,7 +2255,7 @@
       <c r="E8" s="34"/>
       <c r="F8" s="34"/>
       <c r="G8" s="34"/>
-      <c r="H8" s="56"/>
+      <c r="H8" s="34"/>
       <c r="I8" s="34"/>
       <c r="J8" s="34"/>
       <c r="K8" s="34"/>
@@ -2194,9 +2282,9 @@
       <c r="E9" s="56"/>
       <c r="F9" s="34"/>
       <c r="G9" s="34"/>
-      <c r="H9" s="56"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="34"/>
-      <c r="J9" s="34"/>
+      <c r="J9" s="56"/>
       <c r="K9" s="34"/>
       <c r="L9" s="34"/>
       <c r="M9" s="34"/>
@@ -2219,7 +2307,7 @@
       <c r="C10" s="34"/>
       <c r="D10" s="34"/>
       <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
+      <c r="F10" s="56"/>
       <c r="G10" s="56"/>
       <c r="H10" s="34"/>
       <c r="I10" s="34"/>
@@ -2250,8 +2338,8 @@
       <c r="G11" s="34"/>
       <c r="H11" s="34"/>
       <c r="I11" s="34"/>
-      <c r="J11" s="34"/>
-      <c r="K11" s="34"/>
+      <c r="J11" s="56"/>
+      <c r="K11" s="56"/>
       <c r="L11" s="34"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
@@ -2321,7 +2409,7 @@
     </row>
     <row r="14" spans="1:23" ht="35" customHeight="1">
       <c r="A14" s="47" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="B14" s="51"/>
       <c r="C14" s="34"/>
@@ -2329,8 +2417,8 @@
       <c r="E14" s="34"/>
       <c r="F14" s="34"/>
       <c r="G14" s="34"/>
-      <c r="H14" s="34"/>
-      <c r="I14" s="34"/>
+      <c r="H14" s="56"/>
+      <c r="I14" s="56"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
       <c r="L14" s="34"/>
@@ -2348,7 +2436,7 @@
     </row>
     <row r="15" spans="1:23" ht="35" customHeight="1">
       <c r="A15" s="47" t="s">
-        <v>16</v>
+        <v>86</v>
       </c>
       <c r="B15" s="51"/>
       <c r="C15" s="34"/>
@@ -2375,17 +2463,17 @@
     </row>
     <row r="16" spans="1:23" ht="35" customHeight="1">
       <c r="A16" s="47" t="s">
-        <v>17</v>
-      </c>
-      <c r="B16" s="58"/>
-      <c r="C16" s="56"/>
-      <c r="D16" s="56"/>
-      <c r="E16" s="56"/>
-      <c r="F16" s="56"/>
+        <v>16</v>
+      </c>
+      <c r="B16" s="51"/>
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="34"/>
+      <c r="F16" s="34"/>
       <c r="G16" s="34"/>
-      <c r="H16" s="56"/>
-      <c r="I16" s="56"/>
-      <c r="J16" s="34"/>
+      <c r="H16" s="34"/>
+      <c r="I16" s="34"/>
+      <c r="J16" s="90"/>
       <c r="K16" s="34"/>
       <c r="L16" s="34"/>
       <c r="M16" s="34"/>
@@ -2402,18 +2490,18 @@
     </row>
     <row r="17" spans="1:23" ht="35" customHeight="1">
       <c r="A17" s="47" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="51"/>
-      <c r="C17" s="34"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
+        <v>17</v>
+      </c>
+      <c r="B17" s="58"/>
+      <c r="C17" s="56"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="34"/>
       <c r="H17" s="34"/>
-      <c r="I17" s="34"/>
-      <c r="J17" s="34"/>
-      <c r="K17" s="34"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="56"/>
+      <c r="K17" s="56"/>
       <c r="L17" s="34"/>
       <c r="M17" s="34"/>
       <c r="N17" s="34"/>
@@ -2429,7 +2517,7 @@
     </row>
     <row r="18" spans="1:23" ht="35" customHeight="1">
       <c r="A18" s="47" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B18" s="51"/>
       <c r="C18" s="34"/>
@@ -2454,35 +2542,71 @@
       <c r="V18" s="34"/>
       <c r="W18" s="52"/>
     </row>
-    <row r="19" spans="1:23" ht="35" customHeight="1" thickBot="1">
-      <c r="A19" s="48" t="s">
+    <row r="19" spans="1:23" ht="35" customHeight="1">
+      <c r="A19" s="47" t="s">
+        <v>19</v>
+      </c>
+      <c r="B19" s="51"/>
+      <c r="C19" s="34"/>
+      <c r="D19" s="34"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34"/>
+      <c r="H19" s="34"/>
+      <c r="I19" s="34"/>
+      <c r="J19" s="34"/>
+      <c r="K19" s="34"/>
+      <c r="L19" s="34"/>
+      <c r="M19" s="34"/>
+      <c r="N19" s="34"/>
+      <c r="O19" s="34"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="34"/>
+      <c r="R19" s="34"/>
+      <c r="S19" s="34"/>
+      <c r="T19" s="34"/>
+      <c r="U19" s="34"/>
+      <c r="V19" s="34"/>
+      <c r="W19" s="52"/>
+    </row>
+    <row r="20" spans="1:23" ht="35" customHeight="1" thickBot="1">
+      <c r="A20" s="48" t="s">
         <v>20</v>
       </c>
-      <c r="B19" s="59"/>
-      <c r="C19" s="57"/>
-      <c r="D19" s="57"/>
-      <c r="E19" s="57"/>
-      <c r="F19" s="57"/>
-      <c r="G19" s="57"/>
-      <c r="H19" s="57"/>
-      <c r="I19" s="57"/>
-      <c r="J19" s="53"/>
-      <c r="K19" s="53"/>
-      <c r="L19" s="53"/>
-      <c r="M19" s="53"/>
-      <c r="N19" s="53"/>
-      <c r="O19" s="53"/>
-      <c r="P19" s="53"/>
-      <c r="Q19" s="53"/>
-      <c r="R19" s="53"/>
-      <c r="S19" s="53"/>
-      <c r="T19" s="53"/>
-      <c r="U19" s="53"/>
-      <c r="V19" s="53"/>
-      <c r="W19" s="54"/>
+      <c r="B20" s="59"/>
+      <c r="C20" s="57"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="57"/>
+      <c r="F20" s="57"/>
+      <c r="G20" s="57"/>
+      <c r="H20" s="57"/>
+      <c r="I20" s="57"/>
+      <c r="J20" s="57"/>
+      <c r="K20" s="57"/>
+      <c r="L20" s="53"/>
+      <c r="M20" s="53"/>
+      <c r="N20" s="53"/>
+      <c r="O20" s="53"/>
+      <c r="P20" s="53"/>
+      <c r="Q20" s="53"/>
+      <c r="R20" s="53"/>
+      <c r="S20" s="53"/>
+      <c r="T20" s="53"/>
+      <c r="U20" s="53"/>
+      <c r="V20" s="53"/>
+      <c r="W20" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F3:L3"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
@@ -2494,15 +2618,6 @@
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2510,10 +2625,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C78FCE7-630C-9647-8181-21056D9A31B5}">
-  <dimension ref="A1:K214"/>
+  <dimension ref="A1:K218"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="D39" sqref="D39"/>
+    <sheetView topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47:A55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2525,12 +2640,12 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="69" t="s">
+      <c r="A1" s="75" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="69"/>
-      <c r="C1" s="69"/>
-      <c r="D1" s="69"/>
+      <c r="B1" s="75"/>
+      <c r="C1" s="75"/>
+      <c r="D1" s="75"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2965,128 +3080,230 @@
       <c r="D37" s="68"/>
     </row>
     <row r="38" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A38" s="8">
+      <c r="A38" s="88">
         <v>43598</v>
       </c>
       <c r="B38" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="C38" s="9"/>
+      <c r="C38" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D38" s="14" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="39" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A39" s="8"/>
+      <c r="A39" s="84"/>
       <c r="B39" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="C39" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D39" s="14"/>
+    </row>
+    <row r="40" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A40" s="84"/>
+      <c r="B40" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="C39" s="9"/>
-      <c r="D39" s="14" t="s">
+      <c r="C40" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D40" s="14" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A40" s="8"/>
-      <c r="B40" s="11"/>
-      <c r="C40" s="9"/>
-      <c r="D40" s="14"/>
-    </row>
     <row r="41" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A41" s="8"/>
-      <c r="B41" s="11"/>
-      <c r="C41" s="9"/>
-      <c r="D41" s="14"/>
+      <c r="A41" s="84"/>
+      <c r="B41" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C41" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D41" s="14" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="42" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A42" s="8"/>
-      <c r="B42" s="11"/>
-      <c r="C42" s="9"/>
-      <c r="D42" s="14"/>
+      <c r="A42" s="84"/>
+      <c r="B42" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C42" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D42" s="14" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="43" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A43" s="8"/>
-      <c r="B43" s="11"/>
-      <c r="C43" s="9"/>
-      <c r="D43" s="14"/>
+      <c r="A43" s="84"/>
+      <c r="B43" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D43" s="14" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="44" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A44" s="8"/>
-      <c r="B44" s="11"/>
-      <c r="C44" s="9"/>
-      <c r="D44" s="14"/>
-    </row>
-    <row r="45" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A45" s="8"/>
-      <c r="B45" s="11"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="14"/>
-    </row>
-    <row r="46" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A46" s="8"/>
-      <c r="B46" s="11"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="14"/>
+      <c r="A44" s="84"/>
+      <c r="B44" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D44" s="14" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A45" s="85"/>
+      <c r="B45" s="89" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D45" s="14" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A46" s="81" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="82"/>
+      <c r="C46" s="67">
+        <f>SUM(C38:C45)</f>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="D46" s="68"/>
     </row>
     <row r="47" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A47" s="8"/>
-      <c r="B47" s="11"/>
-      <c r="C47" s="9"/>
-      <c r="D47" s="14"/>
+      <c r="A47" s="88">
+        <v>43599</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C47" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D47" s="14" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="48" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A48" s="8"/>
-      <c r="B48" s="11"/>
-      <c r="C48" s="9"/>
-      <c r="D48" s="14"/>
+      <c r="A48" s="84"/>
+      <c r="B48" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C48" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D48" s="14" t="s">
+        <v>100</v>
+      </c>
     </row>
     <row r="49" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A49" s="8"/>
-      <c r="B49" s="11"/>
-      <c r="C49" s="9"/>
-      <c r="D49" s="14"/>
+      <c r="A49" s="84"/>
+      <c r="B49" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C49" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D49" s="14" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="50" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A50" s="8"/>
-      <c r="B50" s="11"/>
-      <c r="C50" s="9"/>
-      <c r="D50" s="14"/>
+      <c r="A50" s="84"/>
+      <c r="B50" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C50" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D50" s="14" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="51" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A51" s="8"/>
-      <c r="B51" s="11"/>
-      <c r="C51" s="9"/>
-      <c r="D51" s="14"/>
+      <c r="A51" s="84"/>
+      <c r="B51" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C51" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="D51" s="14" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="52" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A52" s="8"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="9"/>
-      <c r="D52" s="14"/>
+      <c r="A52" s="84"/>
+      <c r="B52" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C52" s="9">
+        <v>3.125E-2</v>
+      </c>
+      <c r="D52" s="14" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="53" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A53" s="8"/>
-      <c r="B53" s="11"/>
-      <c r="C53" s="9"/>
-      <c r="D53" s="14"/>
+      <c r="A53" s="84"/>
+      <c r="B53" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C53" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D53" s="14" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="54" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A54" s="8"/>
-      <c r="B54" s="11"/>
-      <c r="C54" s="9"/>
-      <c r="D54" s="14"/>
-    </row>
-    <row r="55" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A55" s="8"/>
-      <c r="B55" s="11"/>
-      <c r="C55" s="9"/>
+      <c r="A54" s="84"/>
+      <c r="B54" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="C54" s="9">
+        <v>1.0416666666666666E-2</v>
+      </c>
+      <c r="D54" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A55" s="85"/>
+      <c r="B55" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C55" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D55" s="14"/>
     </row>
-    <row r="56" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A56" s="8"/>
-      <c r="B56" s="11"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="14"/>
+    <row r="56" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A56" s="81" t="s">
+        <v>113</v>
+      </c>
+      <c r="B56" s="82"/>
+      <c r="C56" s="67">
+        <f>SUM(C47:C55)</f>
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="D56" s="68"/>
     </row>
     <row r="57" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A57" s="8"/>
@@ -4036,8 +4253,36 @@
       <c r="C214" s="9"/>
       <c r="D214" s="14"/>
     </row>
+    <row r="215" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A215" s="8"/>
+      <c r="B215" s="11"/>
+      <c r="C215" s="9"/>
+      <c r="D215" s="14"/>
+    </row>
+    <row r="216" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A216" s="8"/>
+      <c r="B216" s="11"/>
+      <c r="C216" s="9"/>
+      <c r="D216" s="14"/>
+    </row>
+    <row r="217" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A217" s="8"/>
+      <c r="B217" s="11"/>
+      <c r="C217" s="9"/>
+      <c r="D217" s="14"/>
+    </row>
+    <row r="218" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A218" s="8"/>
+      <c r="B218" s="11"/>
+      <c r="C218" s="9"/>
+      <c r="D218" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="11">
+    <mergeCell ref="A46:B46"/>
+    <mergeCell ref="A38:A45"/>
+    <mergeCell ref="A56:B56"/>
+    <mergeCell ref="A47:A55"/>
     <mergeCell ref="A37:B37"/>
     <mergeCell ref="A28:A36"/>
     <mergeCell ref="A1:D1"/>

</xml_diff>

<commit_message>
Cotroler move robot to object
</commit_message>
<xml_diff>
--- a/Docs/EnzoRoy_Planning_Taches.xlsx
+++ b/Docs/EnzoRoy_Planning_Taches.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enzoroy/Desktop/EnzoRoy_TPI/BotCleaner/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{149AA8F3-AED0-FF41-8AAE-17B8FA9FDB68}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25AC32DA-2196-C249-AE58-7AB3A2AA42A4}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" activeTab="1" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19040" activeTab="2" xr2:uid="{D558695E-749D-7F46-AFB7-06FFFFC7FD3F}"/>
   </bookViews>
   <sheets>
     <sheet name="Planning prévisionnel" sheetId="4" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="137">
   <si>
     <t>Date</t>
   </si>
@@ -401,7 +401,49 @@
     <t>continué la doc., questionnement sur problème résolu le jour 4, piece 3d</t>
   </si>
   <si>
-    <t>documenter le code</t>
+    <t>Total J7</t>
+  </si>
+  <si>
+    <t>recuperation coord objet par streaming output</t>
+  </si>
+  <si>
+    <t>Total J8</t>
+  </si>
+  <si>
+    <t>doc fonction</t>
+  </si>
+  <si>
+    <t>renvoie des coords, orbjet au bord problématique,</t>
+  </si>
+  <si>
+    <t>restructuration, amélioration boucle, lisibilité</t>
+  </si>
+  <si>
+    <t>ajout coord streamingoutput</t>
+  </si>
+  <si>
+    <t>streamin output</t>
+  </si>
+  <si>
+    <t>ajout carre</t>
+  </si>
+  <si>
+    <t>correction bug</t>
+  </si>
+  <si>
+    <t>envoie des coords depuis l analyseur</t>
+  </si>
+  <si>
+    <t>affichage carre</t>
+  </si>
+  <si>
+    <t>relecture</t>
+  </si>
+  <si>
+    <t>contrôle robot automatique</t>
+  </si>
+  <si>
+    <t>Total J9</t>
   </si>
 </sst>
 </file>
@@ -1066,6 +1108,27 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1084,23 +1147,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1108,12 +1159,6 @@
     <xf numFmtId="14" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="34" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1125,9 +1170,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1461,145 +1503,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="72" t="s">
         <v>21</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="79" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="81">
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="76">
         <v>43592</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="82"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="77"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="72" t="s">
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="73" t="s">
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="74"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="81"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="82">
         <v>1</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="75">
+      <c r="C5" s="83"/>
+      <c r="D5" s="82">
         <v>2</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="75">
+      <c r="E5" s="83"/>
+      <c r="F5" s="82">
         <v>3</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="75">
+      <c r="G5" s="83"/>
+      <c r="H5" s="82">
         <v>4</v>
       </c>
-      <c r="I5" s="76"/>
-      <c r="J5" s="75">
+      <c r="I5" s="83"/>
+      <c r="J5" s="82">
         <v>5</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="75">
+      <c r="K5" s="83"/>
+      <c r="L5" s="82">
         <v>6</v>
       </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="75">
+      <c r="M5" s="83"/>
+      <c r="N5" s="82">
         <v>7</v>
       </c>
-      <c r="O5" s="76"/>
-      <c r="P5" s="75">
+      <c r="O5" s="83"/>
+      <c r="P5" s="82">
         <v>8</v>
       </c>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="75">
+      <c r="Q5" s="83"/>
+      <c r="R5" s="82">
         <v>9</v>
       </c>
-      <c r="S5" s="76"/>
-      <c r="T5" s="75">
+      <c r="S5" s="83"/>
+      <c r="T5" s="82">
         <v>10</v>
       </c>
-      <c r="U5" s="76"/>
-      <c r="V5" s="75">
+      <c r="U5" s="83"/>
+      <c r="V5" s="82">
         <v>11</v>
       </c>
-      <c r="W5" s="76"/>
+      <c r="W5" s="83"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -1999,11 +2041,6 @@
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="20">
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="Q2:W2"/>
     <mergeCell ref="B3:E3"/>
     <mergeCell ref="F3:L3"/>
     <mergeCell ref="M3:P3"/>
@@ -2019,6 +2056,11 @@
     <mergeCell ref="T5:U5"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="L5:M5"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="Q2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2028,8 +2070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6779F402-4327-4345-BFB9-00C0C178FF50}">
   <dimension ref="A1:W20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2039,145 +2081,145 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="72" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
-      <c r="E1" s="77"/>
-      <c r="F1" s="77"/>
-      <c r="G1" s="77"/>
-      <c r="H1" s="77"/>
-      <c r="I1" s="77"/>
-      <c r="J1" s="77"/>
-      <c r="K1" s="77"/>
-      <c r="L1" s="77"/>
-      <c r="M1" s="77"/>
-      <c r="N1" s="77"/>
-      <c r="O1" s="77"/>
-      <c r="P1" s="77"/>
-      <c r="Q1" s="77"/>
-      <c r="R1" s="77"/>
-      <c r="S1" s="77"/>
-      <c r="T1" s="77"/>
-      <c r="U1" s="77"/>
-      <c r="V1" s="77"/>
-      <c r="W1" s="77"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
+      <c r="E1" s="72"/>
+      <c r="F1" s="72"/>
+      <c r="G1" s="72"/>
+      <c r="H1" s="72"/>
+      <c r="I1" s="72"/>
+      <c r="J1" s="72"/>
+      <c r="K1" s="72"/>
+      <c r="L1" s="72"/>
+      <c r="M1" s="72"/>
+      <c r="N1" s="72"/>
+      <c r="O1" s="72"/>
+      <c r="P1" s="72"/>
+      <c r="Q1" s="72"/>
+      <c r="R1" s="72"/>
+      <c r="S1" s="72"/>
+      <c r="T1" s="72"/>
+      <c r="U1" s="72"/>
+      <c r="V1" s="72"/>
+      <c r="W1" s="72"/>
     </row>
     <row r="2" spans="1:23" ht="19">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="73" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="79"/>
-      <c r="D2" s="79"/>
-      <c r="E2" s="79"/>
-      <c r="F2" s="80" t="s">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="75" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="80"/>
-      <c r="H2" s="80"/>
-      <c r="I2" s="80"/>
-      <c r="J2" s="80"/>
-      <c r="K2" s="80"/>
-      <c r="L2" s="80"/>
-      <c r="M2" s="79" t="s">
+      <c r="G2" s="75"/>
+      <c r="H2" s="75"/>
+      <c r="I2" s="75"/>
+      <c r="J2" s="75"/>
+      <c r="K2" s="75"/>
+      <c r="L2" s="75"/>
+      <c r="M2" s="74" t="s">
         <v>0</v>
       </c>
-      <c r="N2" s="79"/>
-      <c r="O2" s="79"/>
-      <c r="P2" s="79"/>
-      <c r="Q2" s="81">
+      <c r="N2" s="74"/>
+      <c r="O2" s="74"/>
+      <c r="P2" s="74"/>
+      <c r="Q2" s="76">
         <v>43592</v>
       </c>
-      <c r="R2" s="81"/>
-      <c r="S2" s="81"/>
-      <c r="T2" s="81"/>
-      <c r="U2" s="81"/>
-      <c r="V2" s="81"/>
-      <c r="W2" s="82"/>
+      <c r="R2" s="76"/>
+      <c r="S2" s="76"/>
+      <c r="T2" s="76"/>
+      <c r="U2" s="76"/>
+      <c r="V2" s="76"/>
+      <c r="W2" s="77"/>
     </row>
     <row r="3" spans="1:23" ht="20" thickBot="1">
-      <c r="B3" s="71" t="s">
+      <c r="B3" s="78" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="72"/>
-      <c r="D3" s="72"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="73" t="s">
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="80" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="72" t="s">
+      <c r="G3" s="80"/>
+      <c r="H3" s="80"/>
+      <c r="I3" s="80"/>
+      <c r="J3" s="80"/>
+      <c r="K3" s="80"/>
+      <c r="L3" s="80"/>
+      <c r="M3" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="N3" s="72"/>
-      <c r="O3" s="72"/>
-      <c r="P3" s="72"/>
-      <c r="Q3" s="73" t="s">
+      <c r="N3" s="79"/>
+      <c r="O3" s="79"/>
+      <c r="P3" s="79"/>
+      <c r="Q3" s="80" t="s">
         <v>9</v>
       </c>
-      <c r="R3" s="73"/>
-      <c r="S3" s="73"/>
-      <c r="T3" s="73"/>
-      <c r="U3" s="73"/>
-      <c r="V3" s="73"/>
-      <c r="W3" s="74"/>
+      <c r="R3" s="80"/>
+      <c r="S3" s="80"/>
+      <c r="T3" s="80"/>
+      <c r="U3" s="80"/>
+      <c r="V3" s="80"/>
+      <c r="W3" s="81"/>
     </row>
     <row r="4" spans="1:23" ht="17" thickBot="1"/>
     <row r="5" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A5" s="45" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="75">
+      <c r="B5" s="82">
         <v>1</v>
       </c>
-      <c r="C5" s="76"/>
-      <c r="D5" s="75">
+      <c r="C5" s="83"/>
+      <c r="D5" s="82">
         <v>2</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="75">
+      <c r="E5" s="83"/>
+      <c r="F5" s="82">
         <v>3</v>
       </c>
-      <c r="G5" s="76"/>
-      <c r="H5" s="75">
+      <c r="G5" s="83"/>
+      <c r="H5" s="82">
         <v>4</v>
       </c>
-      <c r="I5" s="76"/>
-      <c r="J5" s="75">
+      <c r="I5" s="83"/>
+      <c r="J5" s="82">
         <v>5</v>
       </c>
-      <c r="K5" s="76"/>
-      <c r="L5" s="75">
+      <c r="K5" s="83"/>
+      <c r="L5" s="82">
         <v>6</v>
       </c>
-      <c r="M5" s="76"/>
-      <c r="N5" s="75">
+      <c r="M5" s="83"/>
+      <c r="N5" s="82">
         <v>7</v>
       </c>
-      <c r="O5" s="76"/>
-      <c r="P5" s="75">
+      <c r="O5" s="83"/>
+      <c r="P5" s="82">
         <v>8</v>
       </c>
-      <c r="Q5" s="76"/>
-      <c r="R5" s="75">
+      <c r="Q5" s="83"/>
+      <c r="R5" s="82">
         <v>9</v>
       </c>
-      <c r="S5" s="76"/>
-      <c r="T5" s="75">
+      <c r="S5" s="83"/>
+      <c r="T5" s="82">
         <v>10</v>
       </c>
-      <c r="U5" s="76"/>
-      <c r="V5" s="75">
+      <c r="U5" s="83"/>
+      <c r="V5" s="82">
         <v>11</v>
       </c>
-      <c r="W5" s="76"/>
+      <c r="W5" s="83"/>
     </row>
     <row r="6" spans="1:23" ht="35" customHeight="1" thickBot="1">
       <c r="A6" s="46" t="s">
@@ -2375,8 +2417,8 @@
       <c r="L11" s="56"/>
       <c r="M11" s="34"/>
       <c r="N11" s="34"/>
-      <c r="O11" s="34"/>
-      <c r="P11" s="34"/>
+      <c r="O11" s="56"/>
+      <c r="P11" s="56"/>
       <c r="Q11" s="34"/>
       <c r="R11" s="34"/>
       <c r="S11" s="34"/>
@@ -2430,10 +2472,10 @@
       <c r="M13" s="34"/>
       <c r="N13" s="34"/>
       <c r="O13" s="34"/>
-      <c r="P13" s="34"/>
+      <c r="P13" s="56"/>
       <c r="Q13" s="34"/>
       <c r="R13" s="34"/>
-      <c r="S13" s="34"/>
+      <c r="S13" s="56"/>
       <c r="T13" s="34"/>
       <c r="U13" s="34"/>
       <c r="V13" s="34"/>
@@ -2453,7 +2495,7 @@
       <c r="I14" s="56"/>
       <c r="J14" s="34"/>
       <c r="K14" s="34"/>
-      <c r="L14" s="34"/>
+      <c r="L14" s="56"/>
       <c r="M14" s="34"/>
       <c r="N14" s="34"/>
       <c r="O14" s="34"/>
@@ -2539,9 +2581,9 @@
       <c r="N17" s="56"/>
       <c r="O17" s="56"/>
       <c r="P17" s="34"/>
-      <c r="Q17" s="34"/>
-      <c r="R17" s="34"/>
-      <c r="S17" s="34"/>
+      <c r="Q17" s="56"/>
+      <c r="R17" s="56"/>
+      <c r="S17" s="56"/>
       <c r="T17" s="34"/>
       <c r="U17" s="34"/>
       <c r="V17" s="34"/>
@@ -2617,12 +2659,12 @@
       <c r="K20" s="57"/>
       <c r="L20" s="57"/>
       <c r="M20" s="57"/>
-      <c r="N20" s="53"/>
-      <c r="O20" s="53"/>
-      <c r="P20" s="53"/>
-      <c r="Q20" s="53"/>
-      <c r="R20" s="53"/>
-      <c r="S20" s="53"/>
+      <c r="N20" s="57"/>
+      <c r="O20" s="57"/>
+      <c r="P20" s="57"/>
+      <c r="Q20" s="57"/>
+      <c r="R20" s="57"/>
+      <c r="S20" s="57"/>
       <c r="T20" s="53"/>
       <c r="U20" s="53"/>
       <c r="V20" s="53"/>
@@ -2630,15 +2672,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="M2:P2"/>
-    <mergeCell ref="M3:P3"/>
-    <mergeCell ref="Q2:W2"/>
-    <mergeCell ref="Q3:W3"/>
-    <mergeCell ref="A1:W1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="B3:E3"/>
-    <mergeCell ref="F2:L2"/>
-    <mergeCell ref="F3:L3"/>
     <mergeCell ref="V5:W5"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="D5:E5"/>
@@ -2650,6 +2683,15 @@
     <mergeCell ref="P5:Q5"/>
     <mergeCell ref="R5:S5"/>
     <mergeCell ref="T5:U5"/>
+    <mergeCell ref="M2:P2"/>
+    <mergeCell ref="M3:P3"/>
+    <mergeCell ref="Q2:W2"/>
+    <mergeCell ref="Q3:W3"/>
+    <mergeCell ref="A1:W1"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="F2:L2"/>
+    <mergeCell ref="F3:L3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2657,27 +2699,27 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C78FCE7-630C-9647-8181-21056D9A31B5}">
-  <dimension ref="A1:K220"/>
+  <dimension ref="A1:K221"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D65" sqref="D65"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="A79" sqref="A79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="5"/>
     <col min="2" max="2" width="34" style="12" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" style="4"/>
+    <col min="3" max="3" width="13.1640625" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="54.5" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="60" customHeight="1" thickBot="1">
-      <c r="A1" s="77" t="s">
+      <c r="A1" s="72" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="77"/>
-      <c r="C1" s="77"/>
-      <c r="D1" s="77"/>
+      <c r="B1" s="72"/>
+      <c r="C1" s="72"/>
+      <c r="D1" s="72"/>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
       <c r="G1" s="2"/>
@@ -2735,7 +2777,7 @@
       </c>
     </row>
     <row r="6" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A6" s="83">
+      <c r="A6" s="86">
         <v>43592</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -2749,7 +2791,7 @@
       </c>
     </row>
     <row r="7" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A7" s="84"/>
+      <c r="A7" s="87"/>
       <c r="B7" s="11" t="s">
         <v>27</v>
       </c>
@@ -2761,7 +2803,7 @@
       </c>
     </row>
     <row r="8" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A8" s="84"/>
+      <c r="A8" s="87"/>
       <c r="B8" s="11" t="s">
         <v>28</v>
       </c>
@@ -2773,7 +2815,7 @@
       </c>
     </row>
     <row r="9" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A9" s="84"/>
+      <c r="A9" s="87"/>
       <c r="B9" s="11" t="s">
         <v>17</v>
       </c>
@@ -2785,7 +2827,7 @@
       </c>
     </row>
     <row r="10" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A10" s="84"/>
+      <c r="A10" s="87"/>
       <c r="B10" s="11" t="s">
         <v>34</v>
       </c>
@@ -2797,7 +2839,7 @@
       </c>
     </row>
     <row r="11" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A11" s="84"/>
+      <c r="A11" s="87"/>
       <c r="B11" s="11" t="s">
         <v>35</v>
       </c>
@@ -2809,7 +2851,7 @@
       </c>
     </row>
     <row r="12" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A12" s="84"/>
+      <c r="A12" s="87"/>
       <c r="B12" s="11" t="s">
         <v>38</v>
       </c>
@@ -2821,7 +2863,7 @@
       </c>
     </row>
     <row r="13" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A13" s="84"/>
+      <c r="A13" s="87"/>
       <c r="B13" s="11" t="s">
         <v>40</v>
       </c>
@@ -2833,7 +2875,7 @@
       </c>
     </row>
     <row r="14" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A14" s="84"/>
+      <c r="A14" s="87"/>
       <c r="B14" s="11" t="s">
         <v>42</v>
       </c>
@@ -2845,7 +2887,7 @@
       </c>
     </row>
     <row r="15" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A15" s="84"/>
+      <c r="A15" s="87"/>
       <c r="B15" s="11" t="s">
         <v>43</v>
       </c>
@@ -2857,7 +2899,7 @@
       </c>
     </row>
     <row r="16" spans="1:11" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A16" s="84"/>
+      <c r="A16" s="87"/>
       <c r="B16" s="11" t="s">
         <v>46</v>
       </c>
@@ -2867,10 +2909,10 @@
       <c r="D16" s="14"/>
     </row>
     <row r="17" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A17" s="89" t="s">
+      <c r="A17" s="90" t="s">
         <v>47</v>
       </c>
-      <c r="B17" s="90"/>
+      <c r="B17" s="91"/>
       <c r="C17" s="63">
         <f>SUM(C6:C16)</f>
         <v>0.32291666666666663</v>
@@ -2878,7 +2920,7 @@
       <c r="D17" s="64"/>
     </row>
     <row r="18" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
-      <c r="A18" s="87">
+      <c r="A18" s="88">
         <v>43593</v>
       </c>
       <c r="B18" s="11" t="s">
@@ -2888,7 +2930,7 @@
       <c r="D18" s="60"/>
     </row>
     <row r="19" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A19" s="84"/>
+      <c r="A19" s="87"/>
       <c r="B19" s="62" t="s">
         <v>48</v>
       </c>
@@ -2898,7 +2940,7 @@
       <c r="D19" s="14"/>
     </row>
     <row r="20" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A20" s="84"/>
+      <c r="A20" s="87"/>
       <c r="B20" s="62" t="s">
         <v>49</v>
       </c>
@@ -2908,7 +2950,7 @@
       <c r="D20" s="14"/>
     </row>
     <row r="21" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A21" s="84"/>
+      <c r="A21" s="87"/>
       <c r="B21" s="62" t="s">
         <v>50</v>
       </c>
@@ -2920,7 +2962,7 @@
       </c>
     </row>
     <row r="22" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A22" s="84"/>
+      <c r="A22" s="87"/>
       <c r="B22" s="11" t="s">
         <v>52</v>
       </c>
@@ -2932,7 +2974,7 @@
       </c>
     </row>
     <row r="23" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A23" s="84"/>
+      <c r="A23" s="87"/>
       <c r="B23" s="11" t="s">
         <v>54</v>
       </c>
@@ -2944,7 +2986,7 @@
       </c>
     </row>
     <row r="24" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A24" s="84"/>
+      <c r="A24" s="87"/>
       <c r="B24" s="11" t="s">
         <v>56</v>
       </c>
@@ -2956,19 +2998,19 @@
       </c>
     </row>
     <row r="25" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A25" s="84"/>
+      <c r="A25" s="87"/>
       <c r="B25" s="11" t="s">
         <v>58</v>
       </c>
       <c r="C25" s="9">
-        <v>3.125E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D25" s="14" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="26" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A26" s="88"/>
+      <c r="A26" s="89"/>
       <c r="B26" s="11" t="s">
         <v>59</v>
       </c>
@@ -2980,18 +3022,18 @@
       </c>
     </row>
     <row r="27" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A27" s="89" t="s">
+      <c r="A27" s="90" t="s">
         <v>62</v>
       </c>
-      <c r="B27" s="90"/>
+      <c r="B27" s="91"/>
       <c r="C27" s="63">
         <f>SUM(C19:C26)</f>
-        <v>0.32291666666666669</v>
+        <v>0.33333333333333337</v>
       </c>
       <c r="D27" s="65"/>
     </row>
     <row r="28" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1">
-      <c r="A28" s="87">
+      <c r="A28" s="88">
         <v>43594</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -3005,7 +3047,7 @@
       </c>
     </row>
     <row r="29" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A29" s="84"/>
+      <c r="A29" s="87"/>
       <c r="B29" s="11" t="s">
         <v>54</v>
       </c>
@@ -3017,7 +3059,7 @@
       </c>
     </row>
     <row r="30" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A30" s="84"/>
+      <c r="A30" s="87"/>
       <c r="B30" s="11" t="s">
         <v>66</v>
       </c>
@@ -3029,7 +3071,7 @@
       </c>
     </row>
     <row r="31" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A31" s="84"/>
+      <c r="A31" s="87"/>
       <c r="B31" s="11" t="s">
         <v>68</v>
       </c>
@@ -3041,7 +3083,7 @@
       </c>
     </row>
     <row r="32" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A32" s="84"/>
+      <c r="A32" s="87"/>
       <c r="B32" s="11" t="s">
         <v>70</v>
       </c>
@@ -3053,7 +3095,7 @@
       </c>
     </row>
     <row r="33" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A33" s="84"/>
+      <c r="A33" s="87"/>
       <c r="B33" s="11" t="s">
         <v>71</v>
       </c>
@@ -3065,7 +3107,7 @@
       </c>
     </row>
     <row r="34" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A34" s="84"/>
+      <c r="A34" s="87"/>
       <c r="B34" s="11" t="s">
         <v>77</v>
       </c>
@@ -3077,19 +3119,19 @@
       </c>
     </row>
     <row r="35" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A35" s="84"/>
+      <c r="A35" s="87"/>
       <c r="B35" s="11" t="s">
         <v>74</v>
       </c>
       <c r="C35" s="9">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D35" s="14" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="36" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A36" s="84"/>
+      <c r="A36" s="87"/>
       <c r="B36" s="11" t="s">
         <v>75</v>
       </c>
@@ -3101,8 +3143,8 @@
       </c>
     </row>
     <row r="37" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A37" s="88"/>
-      <c r="B37" s="91" t="s">
+      <c r="A37" s="89"/>
+      <c r="B37" s="71" t="s">
         <v>99</v>
       </c>
       <c r="C37" s="9">
@@ -3113,18 +3155,18 @@
       </c>
     </row>
     <row r="38" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A38" s="85" t="s">
+      <c r="A38" s="84" t="s">
         <v>80</v>
       </c>
-      <c r="B38" s="86"/>
+      <c r="B38" s="85"/>
       <c r="C38" s="67">
         <f>SUM(C28:C37)</f>
-        <v>0.31249999999999994</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D38" s="68"/>
     </row>
     <row r="39" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A39" s="83">
+      <c r="A39" s="86">
         <v>43598</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -3138,7 +3180,7 @@
       </c>
     </row>
     <row r="40" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A40" s="84"/>
+      <c r="A40" s="87"/>
       <c r="B40" s="11" t="s">
         <v>17</v>
       </c>
@@ -3148,19 +3190,19 @@
       <c r="D40" s="14"/>
     </row>
     <row r="41" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A41" s="84"/>
+      <c r="A41" s="87"/>
       <c r="B41" s="11" t="s">
         <v>84</v>
       </c>
       <c r="C41" s="9">
-        <v>2.0833333333333332E-2</v>
+        <v>4.1666666666666664E-2</v>
       </c>
       <c r="D41" s="14" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="42" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A42" s="84"/>
+      <c r="A42" s="87"/>
       <c r="B42" s="11" t="s">
         <v>88</v>
       </c>
@@ -3172,7 +3214,7 @@
       </c>
     </row>
     <row r="43" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A43" s="84"/>
+      <c r="A43" s="87"/>
       <c r="B43" s="11" t="s">
         <v>95</v>
       </c>
@@ -3184,7 +3226,7 @@
       </c>
     </row>
     <row r="44" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A44" s="84"/>
+      <c r="A44" s="87"/>
       <c r="B44" s="11" t="s">
         <v>88</v>
       </c>
@@ -3196,7 +3238,7 @@
       </c>
     </row>
     <row r="45" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A45" s="84"/>
+      <c r="A45" s="87"/>
       <c r="B45" s="11" t="s">
         <v>90</v>
       </c>
@@ -3208,22 +3250,22 @@
       </c>
     </row>
     <row r="46" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A46" s="88"/>
+      <c r="A46" s="89"/>
       <c r="B46" s="69" t="s">
         <v>93</v>
       </c>
       <c r="C46" s="9">
-        <v>4.1666666666666664E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D46" s="14" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="47" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A47" s="85" t="s">
+      <c r="A47" s="84" t="s">
         <v>97</v>
       </c>
-      <c r="B47" s="86"/>
+      <c r="B47" s="85"/>
       <c r="C47" s="67">
         <f>SUM(C39:C46)</f>
         <v>0.29166666666666663</v>
@@ -3231,7 +3273,7 @@
       <c r="D47" s="68"/>
     </row>
     <row r="48" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A48" s="83">
+      <c r="A48" s="86">
         <v>43599</v>
       </c>
       <c r="B48" s="11" t="s">
@@ -3245,7 +3287,7 @@
       </c>
     </row>
     <row r="49" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A49" s="84"/>
+      <c r="A49" s="87"/>
       <c r="B49" s="11" t="s">
         <v>99</v>
       </c>
@@ -3257,7 +3299,7 @@
       </c>
     </row>
     <row r="50" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A50" s="84"/>
+      <c r="A50" s="87"/>
       <c r="B50" s="11" t="s">
         <v>102</v>
       </c>
@@ -3269,7 +3311,7 @@
       </c>
     </row>
     <row r="51" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A51" s="84"/>
+      <c r="A51" s="87"/>
       <c r="B51" s="11" t="s">
         <v>103</v>
       </c>
@@ -3281,7 +3323,7 @@
       </c>
     </row>
     <row r="52" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A52" s="84"/>
+      <c r="A52" s="87"/>
       <c r="B52" s="11" t="s">
         <v>106</v>
       </c>
@@ -3293,19 +3335,19 @@
       </c>
     </row>
     <row r="53" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A53" s="84"/>
+      <c r="A53" s="87"/>
       <c r="B53" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C53" s="9">
-        <v>3.125E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D53" s="14" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="54" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A54" s="84"/>
+      <c r="A54" s="87"/>
       <c r="B54" s="11" t="s">
         <v>108</v>
       </c>
@@ -3317,19 +3359,19 @@
       </c>
     </row>
     <row r="55" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A55" s="84"/>
+      <c r="A55" s="87"/>
       <c r="B55" s="11" t="s">
         <v>107</v>
       </c>
       <c r="C55" s="9">
-        <v>1.0416666666666666E-2</v>
+        <v>2.0833333333333332E-2</v>
       </c>
       <c r="D55" s="14" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="56" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A56" s="88"/>
+      <c r="A56" s="89"/>
       <c r="B56" s="11" t="s">
         <v>108</v>
       </c>
@@ -3339,10 +3381,10 @@
       <c r="D56" s="14"/>
     </row>
     <row r="57" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A57" s="85" t="s">
+      <c r="A57" s="84" t="s">
         <v>113</v>
       </c>
-      <c r="B57" s="86"/>
+      <c r="B57" s="85"/>
       <c r="C57" s="67">
         <f>SUM(C48:C56)</f>
         <v>0.30208333333333331</v>
@@ -3350,7 +3392,7 @@
       <c r="D57" s="68"/>
     </row>
     <row r="58" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A58" s="83">
+      <c r="A58" s="86">
         <v>43600</v>
       </c>
       <c r="B58" s="11" t="s">
@@ -3364,28 +3406,28 @@
       </c>
     </row>
     <row r="59" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A59" s="84"/>
+      <c r="A59" s="87"/>
       <c r="B59" s="11" t="s">
-        <v>98</v>
+        <v>46</v>
       </c>
       <c r="C59" s="9">
-        <v>0.14583333333333334</v>
+        <v>0.16666666666666666</v>
       </c>
       <c r="D59" s="14"/>
     </row>
     <row r="60" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A60" s="85" t="s">
+      <c r="A60" s="84" t="s">
         <v>116</v>
       </c>
-      <c r="B60" s="86"/>
+      <c r="B60" s="85"/>
       <c r="C60" s="67">
         <f>SUM(C58:C59)</f>
-        <v>0.3125</v>
+        <v>0.33333333333333331</v>
       </c>
       <c r="D60" s="68"/>
     </row>
     <row r="61" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A61" s="8">
+      <c r="A61" s="86">
         <v>43601</v>
       </c>
       <c r="B61" s="11" t="s">
@@ -3397,7 +3439,7 @@
       <c r="D61" s="14"/>
     </row>
     <row r="62" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A62" s="70"/>
+      <c r="A62" s="87"/>
       <c r="B62" s="11" t="s">
         <v>108</v>
       </c>
@@ -3409,7 +3451,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A63" s="8"/>
+      <c r="A63" s="87"/>
       <c r="B63" s="11" t="s">
         <v>66</v>
       </c>
@@ -3421,7 +3463,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A64" s="8"/>
+      <c r="A64" s="87"/>
       <c r="B64" s="11" t="s">
         <v>119</v>
       </c>
@@ -3429,11 +3471,11 @@
         <v>8.3333333333333329E-2</v>
       </c>
       <c r="D64" s="14" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
-      <c r="A65" s="8"/>
+      <c r="A65" s="89"/>
       <c r="B65" s="11" t="s">
         <v>118</v>
       </c>
@@ -3443,10 +3485,10 @@
       <c r="D65" s="14"/>
     </row>
     <row r="66" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
-      <c r="A66" s="85" t="s">
-        <v>116</v>
-      </c>
-      <c r="B66" s="86"/>
+      <c r="A66" s="84" t="s">
+        <v>122</v>
+      </c>
+      <c r="B66" s="85"/>
       <c r="C66" s="67">
         <f>SUM(C61:C65)</f>
         <v>0.3125</v>
@@ -3454,76 +3496,144 @@
       <c r="D66" s="68"/>
     </row>
     <row r="67" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A67" s="8"/>
-      <c r="B67" s="11"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="14"/>
+      <c r="A67" s="86">
+        <v>43605</v>
+      </c>
+      <c r="B67" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="C67" s="9">
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D67" s="14" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="68" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A68" s="8"/>
-      <c r="B68" s="11"/>
-      <c r="C68" s="9"/>
-      <c r="D68" s="14"/>
+      <c r="A68" s="87"/>
+      <c r="B68" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C68" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D68" s="14" t="s">
+        <v>127</v>
+      </c>
     </row>
     <row r="69" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A69" s="8"/>
-      <c r="B69" s="11"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="14"/>
-    </row>
-    <row r="70" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A70" s="8"/>
-      <c r="B70" s="11"/>
-      <c r="C70" s="9"/>
+      <c r="A69" s="87"/>
+      <c r="B69" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="C69" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D69" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
+      <c r="A70" s="89"/>
+      <c r="B70" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="C70" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D70" s="14"/>
     </row>
-    <row r="71" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A71" s="8"/>
-      <c r="B71" s="11"/>
-      <c r="C71" s="9"/>
-      <c r="D71" s="14"/>
+    <row r="71" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A71" s="84" t="s">
+        <v>124</v>
+      </c>
+      <c r="B71" s="85"/>
+      <c r="C71" s="67">
+        <f>SUM(C67:C70)</f>
+        <v>0.29166666666666663</v>
+      </c>
+      <c r="D71" s="68"/>
     </row>
     <row r="72" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A72" s="8"/>
-      <c r="B72" s="11"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="14"/>
+      <c r="A72" s="70">
+        <v>43606</v>
+      </c>
+      <c r="B72" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="C72" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D72" s="14" t="s">
+        <v>130</v>
+      </c>
     </row>
     <row r="73" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A73" s="8"/>
-      <c r="B73" s="11"/>
-      <c r="C73" s="9"/>
-      <c r="D73" s="14"/>
+      <c r="A73" s="70"/>
+      <c r="B73" s="11" t="s">
+        <v>131</v>
+      </c>
+      <c r="C73" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D73" s="14" t="s">
+        <v>132</v>
+      </c>
     </row>
     <row r="74" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A74" s="8"/>
-      <c r="B74" s="11"/>
-      <c r="C74" s="9"/>
+      <c r="B74" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="C74" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
       <c r="D74" s="14"/>
     </row>
     <row r="75" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A75" s="8"/>
-      <c r="B75" s="11"/>
-      <c r="C75" s="9"/>
-      <c r="D75" s="14"/>
+      <c r="A75" s="70"/>
+      <c r="B75" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C75" s="9">
+        <v>4.1666666666666664E-2</v>
+      </c>
+      <c r="D75" s="14" t="s">
+        <v>133</v>
+      </c>
     </row>
     <row r="76" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A76" s="8"/>
-      <c r="B76" s="11"/>
-      <c r="C76" s="9"/>
-      <c r="D76" s="14"/>
-    </row>
-    <row r="77" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="B76" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="C76" s="9">
+        <v>6.25E-2</v>
+      </c>
+      <c r="D76" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickBot="1">
       <c r="A77" s="8"/>
-      <c r="B77" s="11"/>
-      <c r="C77" s="9"/>
+      <c r="B77" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="C77" s="9">
+        <v>2.0833333333333332E-2</v>
+      </c>
       <c r="D77" s="14"/>
     </row>
-    <row r="78" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
-      <c r="A78" s="8"/>
-      <c r="B78" s="11"/>
-      <c r="C78" s="9"/>
-      <c r="D78" s="14"/>
+    <row r="78" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1" thickTop="1" thickBot="1">
+      <c r="A78" s="84" t="s">
+        <v>136</v>
+      </c>
+      <c r="B78" s="85"/>
+      <c r="C78" s="67">
+        <f>SUM(C72:C77)</f>
+        <v>0.27083333333333331</v>
+      </c>
+      <c r="D78" s="68"/>
     </row>
     <row r="79" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
       <c r="A79" s="8"/>
@@ -4377,8 +4487,17 @@
       <c r="C220" s="9"/>
       <c r="D220" s="14"/>
     </row>
+    <row r="221" spans="1:4" s="7" customFormat="1" ht="32" customHeight="1">
+      <c r="A221" s="8"/>
+      <c r="B221" s="11"/>
+      <c r="C221" s="9"/>
+      <c r="D221" s="14"/>
+    </row>
   </sheetData>
-  <mergeCells count="14">
+  <mergeCells count="18">
+    <mergeCell ref="A78:B78"/>
+    <mergeCell ref="A71:B71"/>
+    <mergeCell ref="A67:A70"/>
     <mergeCell ref="A66:B66"/>
     <mergeCell ref="A58:A59"/>
     <mergeCell ref="A60:B60"/>
@@ -4393,6 +4512,7 @@
     <mergeCell ref="A57:B57"/>
     <mergeCell ref="A48:A56"/>
     <mergeCell ref="A38:B38"/>
+    <mergeCell ref="A61:A65"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>